<commit_message>
complete upto  conditional formating and auditing tools
</commit_message>
<xml_diff>
--- a/MS Excell/Basic To Advance.xlsx
+++ b/MS Excell/Basic To Advance.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
     <sheet name="VlookupWithTrim" sheetId="2" r:id="rId2"/>
     <sheet name="AdvanceConditionalFormstting" sheetId="6" r:id="rId3"/>
-    <sheet name="RelativeReference" sheetId="3" r:id="rId4"/>
-    <sheet name="AbsoluteReference" sheetId="4" r:id="rId5"/>
-    <sheet name="MixedReference" sheetId="5" r:id="rId6"/>
+    <sheet name="ConditionalFormating" sheetId="7" r:id="rId4"/>
+    <sheet name="AuditingTools" sheetId="8" r:id="rId5"/>
+    <sheet name="RelativeReference" sheetId="3" r:id="rId6"/>
+    <sheet name="AbsoluteReference" sheetId="4" r:id="rId7"/>
+    <sheet name="MixedReference" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -240,6 +242,39 @@
   </si>
   <si>
     <t>3.Highlight column &amp; row</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Data Bars, color scales, Icon Seta, Clear Rules</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Desk</t>
+  </si>
+  <si>
+    <t>Tax Per 100</t>
+  </si>
+  <si>
+    <t>FormulaText()</t>
+  </si>
+  <si>
+    <t>Show Formula</t>
   </si>
 </sst>
 </file>
@@ -249,7 +284,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +308,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -327,7 +370,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,12 +388,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,6 +401,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -371,7 +429,31 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -473,23 +555,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -514,8 +579,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1243,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,10 +1320,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1273,16 +1338,16 @@
       <c r="E3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>5000</v>
       </c>
       <c r="E4" t="s">
@@ -1290,13 +1355,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>25</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>35000</v>
       </c>
     </row>
@@ -1307,7 +1372,7 @@
       <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>400</v>
       </c>
     </row>
@@ -1318,7 +1383,7 @@
       <c r="B7" s="1">
         <v>30</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>350</v>
       </c>
     </row>
@@ -1329,15 +1394,15 @@
       <c r="B8" s="1">
         <v>15</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>1500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1354,13 +1419,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>5000</v>
       </c>
       <c r="E13" t="s">
@@ -1368,13 +1433,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>25</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <v>35000</v>
       </c>
     </row>
@@ -1385,7 +1450,7 @@
       <c r="B15" s="1">
         <v>20</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <v>400</v>
       </c>
     </row>
@@ -1396,7 +1461,7 @@
       <c r="B16" s="1">
         <v>30</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>350</v>
       </c>
     </row>
@@ -1407,15 +1472,15 @@
       <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>1500</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1438,16 +1503,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <v>4000</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <v>5000</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>6000</v>
       </c>
       <c r="F22" t="s">
@@ -1458,16 +1523,16 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <v>32000</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <v>35000</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>40000</v>
       </c>
     </row>
@@ -1475,13 +1540,13 @@
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>300</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="9">
         <v>400</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>550</v>
       </c>
     </row>
@@ -1489,13 +1554,13 @@
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="9">
         <v>200</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <v>350</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>450</v>
       </c>
     </row>
@@ -1503,13 +1568,13 @@
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="9">
         <v>1200</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="9">
         <v>1500</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>2000</v>
       </c>
     </row>
@@ -1520,10 +1585,10 @@
     <mergeCell ref="A20:B20"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A8">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>A4=$E$4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="mobile">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="mobile">
       <formula>NOT(ISERROR(SEARCH("mobile",A4)))</formula>
     </cfRule>
     <cfRule type="expression" priority="16">
@@ -1531,15 +1596,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C8">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>A5=$E$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A17">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>A13=$E$4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="mobile">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="mobile">
       <formula>NOT(ISERROR(SEARCH("mobile",A13)))</formula>
     </cfRule>
     <cfRule type="expression" priority="12">
@@ -1547,18 +1612,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:C17">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>$A13=$E$13</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>A14=$E$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A26">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>A22=$E$4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="mobile">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="mobile">
       <formula>NOT(ISERROR(SEARCH("mobile",A22)))</formula>
     </cfRule>
     <cfRule type="expression" priority="7">
@@ -1566,22 +1631,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:C26">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>A23=$E$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:D26">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>D23=$E$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:D26">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$A22=$F$22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:D26">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>B$21=$G$22</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1591,6 +1656,442 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10">
+        <v>80</v>
+      </c>
+      <c r="C5" s="10">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>30</v>
+      </c>
+      <c r="B6" s="10">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10">
+        <v>30</v>
+      </c>
+      <c r="D6" s="10">
+        <v>90</v>
+      </c>
+      <c r="E6" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10">
+        <v>40</v>
+      </c>
+      <c r="C7" s="10">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10">
+        <v>50</v>
+      </c>
+      <c r="E8" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>60</v>
+      </c>
+      <c r="B9" s="10">
+        <v>60</v>
+      </c>
+      <c r="C9" s="10">
+        <v>60</v>
+      </c>
+      <c r="D9" s="10">
+        <v>60</v>
+      </c>
+      <c r="E9" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>70</v>
+      </c>
+      <c r="B10" s="10">
+        <v>70</v>
+      </c>
+      <c r="C10" s="10">
+        <v>70</v>
+      </c>
+      <c r="D10" s="10">
+        <v>70</v>
+      </c>
+      <c r="E10" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>80</v>
+      </c>
+      <c r="B11" s="10">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10">
+        <v>80</v>
+      </c>
+      <c r="D11" s="10">
+        <v>80</v>
+      </c>
+      <c r="E11" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>90</v>
+      </c>
+      <c r="B12" s="10">
+        <v>90</v>
+      </c>
+      <c r="C12" s="10">
+        <v>90</v>
+      </c>
+      <c r="D12" s="10">
+        <v>90</v>
+      </c>
+      <c r="E12" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>100</v>
+      </c>
+      <c r="B13" s="10">
+        <v>100</v>
+      </c>
+      <c r="C13" s="10">
+        <v>100</v>
+      </c>
+      <c r="D13" s="10">
+        <v>100</v>
+      </c>
+      <c r="E13" s="10">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A4:A13">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3C46B422-09CF-47DA-986C-92603087F660}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B13">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A1CACE68-D121-457B-A33A-58553D6B9754}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D13">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E13">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="5Rating">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3C46B422-09CF-47DA-986C-92603087F660}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A4:A13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A1CACE68-D121-457B-A33A-58553D6B9754}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B4:B13</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="10">
+        <v>123</v>
+      </c>
+      <c r="C2" s="10">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10">
+        <f>B2*C2</f>
+        <v>3075</v>
+      </c>
+      <c r="E2" s="10">
+        <f>$B$7*D2</f>
+        <v>246</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E2)</f>
+        <v>=$B$7*D2</v>
+      </c>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="10">
+        <v>103</v>
+      </c>
+      <c r="C3" s="10">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D4" si="0">B3*C3</f>
+        <v>3090</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E4" si="1">$B$7*D3</f>
+        <v>247.20000000000002</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H4" ca="1" si="2">_xlfn.FORMULATEXT(E3)</f>
+        <v>=$B$7*D3</v>
+      </c>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="10">
+        <v>85</v>
+      </c>
+      <c r="C4" s="10">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>1275</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>=$B$7*D4</v>
+      </c>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1715,7 +2216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1829,7 +2330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1840,14 +2341,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -1868,7 +2369,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="1">
@@ -1896,7 +2397,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1">
         <v>20</v>
       </c>
@@ -1922,7 +2423,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1">
         <v>30</v>
       </c>
@@ -1948,7 +2449,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>40</v>
       </c>
@@ -1974,7 +2475,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1">
         <v>50</v>
       </c>

</xml_diff>